<commit_message>
Fixed inverted x axis on fbx Import removed unnecessary model files Added new showcase scene Entity manager now uses a map for faster look up
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AB9D9F-2258-4CB6-B443-6CC9717551D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EE5554-965D-4F72-B265-82E1A2BB1353}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -927,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3214,7 +3214,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added time sine wave Material Added shitty obj importer
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EE5554-965D-4F72-B265-82E1A2BB1353}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F21A262-02E8-41CB-983C-B7F63620EE03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/noble80/Jose-Graphics-Learnings-of-America-for-Make-Benefit-Glorious-Nation-of-Bolivia.git</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -927,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,15 +1048,19 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1062,11 +1072,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1082,11 +1092,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1115,15 +1129,19 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1152,11 +1170,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1183,23 +1205,27 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1217,11 +1243,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>25</v>
@@ -1248,19 +1278,23 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1282,11 +1316,15 @@
       <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G11" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1307,11 +1345,15 @@
       <c r="D12" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G12" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1357,11 +1399,15 @@
       <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G14" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1496,11 +1542,15 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1657,11 +1707,15 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -1860,11 +1914,15 @@
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -1885,11 +1943,15 @@
       <c r="D38" s="5">
         <v>1</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -1910,11 +1972,15 @@
       <c r="D39" s="5">
         <v>4</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2452,11 +2518,15 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -3214,7 +3284,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added flag shader Fixed timed based input
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F21A262-02E8-41CB-983C-B7F63620EE03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938497D3-9EC3-4DEB-90F7-FDE68AAEFCB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,11 +1072,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1290,11 +1290,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -2151,11 +2151,15 @@
       <c r="D46" s="5">
         <v>2</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -3284,7 +3288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Blinn Phong Added reflective cubemap
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938497D3-9EC3-4DEB-90F7-FDE68AAEFCB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55063AAF-11C7-497A-8855-F852C8804D88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,11 +1072,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1290,11 +1290,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1428,11 +1428,15 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1761,11 +1765,15 @@
       <c r="D30" s="5">
         <v>2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -3288,7 +3296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added bloom, cascaded shadow maps, fixed performance on window resize
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3121B1-65CC-47AF-AA84-680408A952AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068BEEB8-BFA2-4B32-8AD0-A1A2AF870174}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Apply multitexturing or advanced texturing techniques to drawn geometry that isn't already in another category.</t>
   </si>
   <si>
-    <t>YOU CAN ADD TEACHER APPROVED FEATURES IN WHITE AREA UNDER APPROPRIATE CATEORIES</t>
-  </si>
-  <si>
     <t>GEOMETRY (features can only be achieved on 1 milestone)</t>
   </si>
   <si>
@@ -349,6 +346,12 @@
   </si>
   <si>
     <t>Gamma correction</t>
+  </si>
+  <si>
+    <t>Cascaded Shadow Maps</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -942,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,7 +965,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -978,7 +981,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1041,12 +1044,12 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="5">
         <v>4</v>
@@ -1058,10 +1061,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
@@ -1073,7 +1076,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1081,16 +1084,16 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -1102,10 +1105,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
@@ -1122,12 +1125,12 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5">
         <v>4</v>
@@ -1139,10 +1142,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
@@ -1150,7 +1153,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1163,7 +1166,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1180,10 +1183,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
@@ -1215,10 +1218,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
@@ -1234,7 +1237,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1253,10 +1256,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
@@ -1288,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
@@ -1299,15 +1302,15 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1326,10 +1329,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G11" s="16">
         <f t="shared" si="0"/>
@@ -1343,7 +1346,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="5">
         <v>4</v>
@@ -1355,10 +1358,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G12" s="16">
         <f t="shared" si="0"/>
@@ -1372,7 +1375,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -1397,7 +1400,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
@@ -1409,10 +1412,10 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G14" s="16">
         <f t="shared" si="0"/>
@@ -1438,10 +1441,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
@@ -1472,16 +1475,26 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G17" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1508,7 +1521,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1520,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G19" s="16">
         <f t="shared" si="0"/>
@@ -1568,10 +1581,10 @@
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
@@ -1646,11 +1659,15 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1660,7 +1677,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="5">
         <v>2</v>
@@ -1685,7 +1702,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -1697,10 +1714,10 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G26" s="16">
         <f t="shared" si="0"/>
@@ -1714,7 +1731,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1733,7 +1750,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" s="5">
         <v>3</v>
@@ -1745,10 +1762,10 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
@@ -1762,7 +1779,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -1787,7 +1804,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="5">
         <v>3</v>
@@ -1799,10 +1816,10 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
@@ -1816,7 +1833,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="5">
         <v>4</v>
@@ -1841,7 +1858,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="5">
         <v>2</v>
@@ -1866,7 +1883,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="5">
         <v>3</v>
@@ -1891,7 +1908,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" s="1">
         <v>2</v>
@@ -1903,10 +1920,10 @@
         <v>2</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G34" s="16">
         <f t="shared" si="0"/>
@@ -1937,7 +1954,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1956,7 +1973,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="5">
         <v>3</v>
@@ -1968,10 +1985,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
@@ -1985,7 +2002,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
@@ -1997,10 +2014,10 @@
         <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
@@ -2014,7 +2031,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="5">
         <v>4</v>
@@ -2026,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
@@ -2043,7 +2060,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="5">
         <v>4</v>
@@ -2143,7 +2160,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -2193,7 +2210,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -2205,10 +2222,10 @@
         <v>2</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
@@ -2275,7 +2292,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="5">
         <v>3</v>
@@ -2325,7 +2342,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="5">
         <v>4</v>
@@ -2350,7 +2367,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="5">
         <v>4</v>
@@ -2411,7 +2428,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="5">
         <v>2</v>
@@ -2436,7 +2453,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="5">
         <v>2</v>
@@ -2447,11 +2464,15 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2461,7 +2482,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" s="5">
         <v>3</v>
@@ -2564,7 +2585,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" s="5">
         <v>2</v>
@@ -2576,10 +2597,10 @@
         <v>2</v>
       </c>
       <c r="E63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
@@ -2593,7 +2614,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -2618,7 +2639,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -2643,7 +2664,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B66" s="5">
         <v>1</v>
@@ -2668,7 +2689,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B67" s="5">
         <v>4</v>
@@ -2771,7 +2792,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B72" s="5">
         <v>2</v>
@@ -2782,11 +2803,15 @@
       <c r="D72" s="5">
         <v>2</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="3"/>
+      <c r="E72" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G72" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
@@ -2796,7 +2821,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -2807,11 +2832,15 @@
       <c r="D73" s="5">
         <v>1</v>
       </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="3"/>
+      <c r="E73" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G73" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
@@ -2821,7 +2850,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B74" s="5">
         <v>2</v>
@@ -2846,7 +2875,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B75" s="5">
         <v>3</v>
@@ -2857,11 +2886,15 @@
       <c r="D75" s="5">
         <v>3</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3"/>
+      <c r="E75" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G75" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -2871,7 +2904,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B76" s="5">
         <v>2</v>
@@ -2896,7 +2929,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B77" s="5">
         <v>3</v>
@@ -2921,7 +2954,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="5">
         <v>3</v>
@@ -2932,11 +2965,15 @@
       <c r="D78" s="5">
         <v>3</v>
       </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="3"/>
+      <c r="E78" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G78" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
@@ -2980,7 +3017,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -2999,7 +3036,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -3020,7 +3057,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -3041,7 +3078,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -3062,7 +3099,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -3083,7 +3120,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -3104,7 +3141,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -3188,7 +3225,9 @@
       <c r="B91" s="6">
         <v>2</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -3206,7 +3245,9 @@
       <c r="B92" s="6">
         <v>1</v>
       </c>
-      <c r="C92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
@@ -3341,7 +3382,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added render to texture Added post process controls Added readme
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068BEEB8-BFA2-4B32-8AD0-A1A2AF870174}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1187C58E-BD84-4FF9-BC89-DEC45C4A8463}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="4788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -528,7 +528,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -542,29 +542,26 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -573,27 +570,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -945,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,7 +961,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="5"/>
@@ -980,7 +977,7 @@
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -992,7 +989,7 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1018,7 +1015,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
@@ -1048,7 +1045,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B4" s="5">
@@ -1066,33 +1063,33 @@
       <c r="F4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
         <v>4</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
         <v>20</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>18</v>
-      </c>
-      <c r="J4" s="17">
+        <v>20</v>
+      </c>
+      <c r="J4" s="16">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
         <v>0</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="16">
         <f>SUM(H6,I6,J6)</f>
-        <v>40</v>
-      </c>
-      <c r="L4" s="17">
+        <v>45</v>
+      </c>
+      <c r="L4" s="16">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="5">
@@ -1110,7 +1107,7 @@
       <c r="F5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1129,7 +1126,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B6" s="5">
@@ -1147,30 +1144,30 @@
       <c r="F6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H6" s="17">
+      <c r="G6" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H6" s="16">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
         <v>40</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="16">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="17">
+        <v>5</v>
+      </c>
+      <c r="J6" s="16">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
         <v>0</v>
       </c>
       <c r="K6" s="5"/>
-      <c r="L6" s="15">
+      <c r="L6" s="14">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="5">
@@ -1188,7 +1185,7 @@
       <c r="F7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1205,7 +1202,7 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="5">
@@ -1223,19 +1220,19 @@
       <c r="F8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H8" s="18">
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="17">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
         <v>20</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
         <v>20</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
         <v>20</v>
       </c>
@@ -1243,7 +1240,7 @@
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="5">
@@ -1261,24 +1258,24 @@
       <c r="F9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="18" t="s">
         <v>25</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="5">
@@ -1296,27 +1293,27 @@
       <c r="F10" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H10" s="19">
+      <c r="G10" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="18">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>40</v>
-      </c>
-      <c r="I10" s="19">
+        <v>45</v>
+      </c>
+      <c r="I10" s="18">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>38</v>
-      </c>
-      <c r="J10" s="19">
+        <v>45</v>
+      </c>
+      <c r="J10" s="18">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B11" s="5">
@@ -1334,7 +1331,7 @@
       <c r="F11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1345,7 +1342,7 @@
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="5">
@@ -1363,7 +1360,7 @@
       <c r="F12" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1374,7 +1371,7 @@
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="5">
@@ -1388,7 +1385,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1399,7 +1396,7 @@
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="5">
@@ -1417,7 +1414,7 @@
       <c r="F14" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1428,7 +1425,7 @@
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="5">
@@ -1446,7 +1443,7 @@
       <c r="F15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1457,13 +1454,13 @@
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="16">
+      <c r="G16" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1474,7 +1471,7 @@
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B17" s="1">
@@ -1492,7 +1489,7 @@
       <c r="F17" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1503,13 +1500,13 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="16">
+      <c r="G18" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1520,7 +1517,7 @@
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B19" s="1">
@@ -1538,7 +1535,7 @@
       <c r="F19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1549,7 +1546,7 @@
       <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="5"/>
@@ -1557,7 +1554,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="16">
+      <c r="G20" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1568,7 +1565,7 @@
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="5">
@@ -1586,7 +1583,7 @@
       <c r="F21" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1597,7 +1594,7 @@
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="5">
@@ -1611,7 +1608,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="16">
+      <c r="G22" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1622,7 +1619,7 @@
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="5">
@@ -1634,11 +1631,15 @@
       <c r="D23" s="5">
         <v>4</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1647,7 +1648,7 @@
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="5">
@@ -1665,7 +1666,7 @@
       <c r="F24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1676,7 +1677,7 @@
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="5">
@@ -1690,7 +1691,7 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="16">
+      <c r="G25" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1701,7 +1702,7 @@
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B26" s="1">
@@ -1719,7 +1720,7 @@
       <c r="F26" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1730,7 +1731,7 @@
       <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B27" s="5"/>
@@ -1738,7 +1739,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="16">
+      <c r="G27" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1749,7 +1750,7 @@
       <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="5">
@@ -1767,7 +1768,7 @@
       <c r="F28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1778,7 +1779,7 @@
       <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="5">
@@ -1792,7 +1793,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="16">
+      <c r="G29" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1803,7 +1804,7 @@
       <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="5">
@@ -1821,7 +1822,7 @@
       <c r="F30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1832,7 +1833,7 @@
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="5">
@@ -1846,7 +1847,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="16">
+      <c r="G31" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1857,7 +1858,7 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="5">
@@ -1871,7 +1872,7 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="16">
+      <c r="G32" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1882,7 +1883,7 @@
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="5">
@@ -1896,7 +1897,7 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="16">
+      <c r="G33" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1907,7 +1908,7 @@
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B34" s="1">
@@ -1925,7 +1926,7 @@
       <c r="F34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1936,13 +1937,13 @@
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="2"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="16">
+      <c r="G35" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1953,7 +1954,7 @@
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="5"/>
@@ -1961,7 +1962,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="2"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="16">
+      <c r="G36" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1972,7 +1973,7 @@
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="19" t="s">
         <v>75</v>
       </c>
       <c r="B37" s="5">
@@ -1990,7 +1991,7 @@
       <c r="F37" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2001,7 +2002,7 @@
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="5">
@@ -2019,7 +2020,7 @@
       <c r="F38" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G38" s="16">
+      <c r="G38" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2030,7 +2031,7 @@
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="9" t="s">
         <v>97</v>
       </c>
       <c r="B39" s="5">
@@ -2048,7 +2049,7 @@
       <c r="F39" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G39" s="16">
+      <c r="G39" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2059,7 +2060,7 @@
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B40" s="5">
@@ -2073,7 +2074,7 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="16">
+      <c r="G40" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2084,7 +2085,7 @@
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="5">
@@ -2098,7 +2099,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="16">
+      <c r="G41" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2109,7 +2110,7 @@
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="5">
@@ -2123,7 +2124,7 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="16">
+      <c r="G42" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2134,7 +2135,7 @@
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B43" s="5">
@@ -2148,7 +2149,7 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="16">
+      <c r="G43" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2159,7 +2160,7 @@
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B44" s="5">
@@ -2173,7 +2174,7 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="16">
+      <c r="G44" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2184,7 +2185,7 @@
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="5">
@@ -2198,7 +2199,7 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="16">
+      <c r="G45" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2209,7 +2210,7 @@
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>69</v>
       </c>
       <c r="B46" s="1">
@@ -2227,7 +2228,7 @@
       <c r="F46" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G46" s="16">
+      <c r="G46" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2238,13 +2239,13 @@
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="2"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="16">
+      <c r="G47" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2255,13 +2256,13 @@
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="2"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="16">
+      <c r="G48" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2272,7 +2273,7 @@
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="5"/>
@@ -2280,7 +2281,7 @@
       <c r="D49" s="5"/>
       <c r="E49" s="2"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="16">
+      <c r="G49" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2291,7 +2292,7 @@
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B50" s="5">
@@ -2305,7 +2306,7 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="16">
+      <c r="G50" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2316,7 +2317,7 @@
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B51" s="5">
@@ -2330,7 +2331,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="16">
+      <c r="G51" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2341,7 +2342,7 @@
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="5">
@@ -2355,7 +2356,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="16">
+      <c r="G52" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2366,7 +2367,7 @@
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B53" s="5">
@@ -2380,7 +2381,7 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="16">
+      <c r="G53" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2391,13 +2392,13 @@
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
+      <c r="A54" s="7"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="2"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="16">
+      <c r="G54" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2408,7 +2409,7 @@
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="5"/>
@@ -2416,7 +2417,7 @@
       <c r="D55" s="5"/>
       <c r="E55" s="2"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="16">
+      <c r="G55" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2427,7 +2428,7 @@
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B56" s="5">
@@ -2441,7 +2442,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="16">
+      <c r="G56" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2452,7 +2453,7 @@
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5">
@@ -2470,7 +2471,7 @@
       <c r="F57" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G57" s="16">
+      <c r="G57" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2481,7 +2482,7 @@
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B58" s="5">
@@ -2495,7 +2496,7 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="16">
+      <c r="G58" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2506,7 +2507,7 @@
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B59" s="5">
@@ -2520,7 +2521,7 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="16">
+      <c r="G59" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2531,13 +2532,13 @@
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="8"/>
+      <c r="A60" s="7"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="2"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="16">
+      <c r="G60" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2548,13 +2549,13 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="8"/>
+      <c r="A61" s="7"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="2"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="16">
+      <c r="G61" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2565,7 +2566,7 @@
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="5"/>
@@ -2573,7 +2574,7 @@
       <c r="D62" s="5"/>
       <c r="E62" s="2"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="16">
+      <c r="G62" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2584,7 +2585,7 @@
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B63" s="5">
@@ -2602,7 +2603,7 @@
       <c r="F63" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G63" s="16">
+      <c r="G63" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2613,7 +2614,7 @@
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="19" t="s">
         <v>98</v>
       </c>
       <c r="B64" s="5">
@@ -2627,7 +2628,7 @@
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="16">
+      <c r="G64" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2638,7 +2639,7 @@
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="19" t="s">
         <v>84</v>
       </c>
       <c r="B65" s="5">
@@ -2652,7 +2653,7 @@
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="16">
+      <c r="G65" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2663,7 +2664,7 @@
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B66" s="5">
@@ -2677,7 +2678,7 @@
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="16">
+      <c r="G66" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2688,7 +2689,7 @@
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B67" s="5">
@@ -2702,7 +2703,7 @@
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="16">
+      <c r="G67" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2713,7 +2714,7 @@
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B68" s="5">
@@ -2727,7 +2728,7 @@
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="16">
+      <c r="G68" s="15">
         <f t="shared" ref="G68:G89" si="1" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
         <v>0</v>
       </c>
@@ -2738,13 +2739,13 @@
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="8"/>
+      <c r="A69" s="7"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="2"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="16">
+      <c r="G69" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2755,13 +2756,13 @@
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A70" s="8"/>
+      <c r="A70" s="7"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="16">
+      <c r="G70" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2772,7 +2773,7 @@
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B71" s="5"/>
@@ -2780,7 +2781,7 @@
       <c r="D71" s="5"/>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="16">
+      <c r="G71" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2791,7 +2792,7 @@
       <c r="L71" s="5"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B72" s="5">
@@ -2809,7 +2810,7 @@
       <c r="F72" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G72" s="16">
+      <c r="G72" s="15">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2820,7 +2821,7 @@
       <c r="L72" s="5"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="10" t="s">
         <v>94</v>
       </c>
       <c r="B73" s="5">
@@ -2838,7 +2839,7 @@
       <c r="F73" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G73" s="16">
+      <c r="G73" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2849,7 +2850,7 @@
       <c r="L73" s="5"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="10" t="s">
         <v>89</v>
       </c>
       <c r="B74" s="5">
@@ -2863,7 +2864,7 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="16">
+      <c r="G74" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2874,7 +2875,7 @@
       <c r="L74" s="5"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B75" s="5">
@@ -2892,7 +2893,7 @@
       <c r="F75" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G75" s="16">
+      <c r="G75" s="15">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2903,7 +2904,7 @@
       <c r="L75" s="5"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B76" s="5">
@@ -2917,7 +2918,7 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="16">
+      <c r="G76" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2928,7 +2929,7 @@
       <c r="L76" s="5"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B77" s="5">
@@ -2942,7 +2943,7 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="16">
+      <c r="G77" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2953,7 +2954,7 @@
       <c r="L77" s="5"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B78" s="5">
@@ -2971,7 +2972,7 @@
       <c r="F78" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G78" s="16">
+      <c r="G78" s="15">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2982,13 +2983,13 @@
       <c r="L78" s="5"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="11"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="2"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="16">
+      <c r="G79" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2999,13 +3000,13 @@
       <c r="L79" s="5"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="11"/>
+      <c r="A80" s="10"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="2"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="16">
+      <c r="G80" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3016,7 +3017,7 @@
       <c r="L80" s="5"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B81" s="5"/>
@@ -3024,7 +3025,7 @@
       <c r="D81" s="5"/>
       <c r="E81" s="2"/>
       <c r="F81" s="3"/>
-      <c r="G81" s="16">
+      <c r="G81" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3035,7 +3036,7 @@
       <c r="L81" s="5"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B82" s="5"/>
@@ -3045,7 +3046,7 @@
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="16">
+      <c r="G82" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3056,7 +3057,7 @@
       <c r="L82" s="5"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B83" s="5"/>
@@ -3066,7 +3067,7 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="16">
+      <c r="G83" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3077,7 +3078,7 @@
       <c r="L83" s="5"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="10" t="s">
         <v>85</v>
       </c>
       <c r="B84" s="5"/>
@@ -3087,7 +3088,7 @@
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="16">
+      <c r="G84" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3098,7 +3099,7 @@
       <c r="L84" s="5"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B85" s="5"/>
@@ -3108,7 +3109,7 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="16">
+      <c r="G85" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3119,7 +3120,7 @@
       <c r="L85" s="5"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="10" t="s">
         <v>57</v>
       </c>
       <c r="B86" s="5"/>
@@ -3129,7 +3130,7 @@
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="16">
+      <c r="G86" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3140,7 +3141,7 @@
       <c r="L86" s="5"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B87" s="5"/>
@@ -3150,7 +3151,7 @@
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="16">
+      <c r="G87" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3161,13 +3162,13 @@
       <c r="L87" s="5"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A88" s="8"/>
+      <c r="A88" s="7"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="2"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="16">
+      <c r="G88" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3178,13 +3179,13 @@
       <c r="L88" s="5"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="8"/>
+      <c r="A89" s="7"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="2"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="16">
+      <c r="G89" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3195,7 +3196,7 @@
       <c r="L89" s="5"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B90" s="4" t="s">
@@ -3213,67 +3214,71 @@
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
-      <c r="I90" s="6"/>
-      <c r="J90" s="6"/>
-      <c r="K90" s="6"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
       <c r="L90" s="5"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="5">
         <v>2</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="6"/>
-      <c r="K91" s="6"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
       <c r="L91" s="5"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="5">
         <v>1</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
-      <c r="I92" s="6"/>
-      <c r="J92" s="6"/>
-      <c r="K92" s="6"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
       <c r="L92" s="5"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="11"/>
+      <c r="A93" s="10"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6"/>
-      <c r="I93" s="6"/>
-      <c r="J93" s="6"/>
-      <c r="K93" s="6"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
       <c r="L93" s="5"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="11"/>
+      <c r="A94" s="10"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -3287,78 +3292,78 @@
       <c r="L94" s="5"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="12"/>
+      <c r="A96" s="11"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="12"/>
+      <c r="A97" s="11"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="12"/>
+      <c r="A98" s="11"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="12"/>
+      <c r="A99" s="11"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="12"/>
+      <c r="A100" s="11"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="12"/>
+      <c r="A101" s="11"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="12"/>
+      <c r="A102" s="11"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="12"/>
+      <c r="A103" s="11"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="12"/>
+      <c r="A104" s="11"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="12"/>
+      <c r="A105" s="11"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="12"/>
+      <c r="A106" s="11"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="12"/>
+      <c r="A107" s="11"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="12"/>
+      <c r="A108" s="11"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="12"/>
+      <c r="A109" s="11"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="12"/>
+      <c r="A110" s="11"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="12"/>
+      <c r="A111" s="11"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="12"/>
+      <c r="A112" s="11"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="12"/>
+      <c r="A113" s="11"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="12"/>
+      <c r="A114" s="11"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="12"/>
+      <c r="A115" s="11"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="12"/>
+      <c r="A116" s="11"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="12"/>
+      <c r="A117" s="11"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="13"/>
+      <c r="A118" s="12"/>
     </row>
   </sheetData>
   <sheetProtection password="A529" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>

</xml_diff>

<commit_message>
Added Fog, DOF, and Screen Warp Refactored depth management in post process chain Readded render to texture flag
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A163F3-F9EC-4E62-9B1E-526E1A6A5F84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C748A0-1A15-4421-ACFD-A3EDB301CC10}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="4788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="110">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -356,6 +355,9 @@
   </si>
   <si>
     <t>Direct3D Rendering Cookbook. Chapter 5: Applying Hardware Tessellation. Barycentric and Bilinear interpolation formulas.</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -946,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,15 +1083,15 @@
       </c>
       <c r="J4" s="16">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K4" s="16">
         <f>SUM(H6,I6,J6)</f>
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="L4" s="16">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1162,12 +1164,12 @@
       </c>
       <c r="J6" s="16">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="14">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1303,15 +1305,15 @@
       </c>
       <c r="H10" s="18">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I10" s="18">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J10" s="18">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1610,11 +1612,15 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G22" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1693,11 +1699,15 @@
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G25" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -2126,11 +2136,15 @@
       <c r="D42" s="5">
         <v>4</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="3"/>
+      <c r="E42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G42" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -2730,11 +2744,15 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G68" s="15">
         <f t="shared" ref="G68:G89" si="1" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -2866,11 +2884,15 @@
       <c r="D74" s="5">
         <v>2</v>
       </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="3"/>
+      <c r="E74" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G74" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
@@ -2920,11 +2942,15 @@
       <c r="D76" s="5">
         <v>2</v>
       </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="3"/>
+      <c r="E76" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G76" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
@@ -2945,11 +2971,15 @@
       <c r="D77" s="5">
         <v>3</v>
       </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="3"/>
+      <c r="E77" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G77" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
@@ -3153,11 +3183,15 @@
       <c r="D87" s="5">
         <v>6</v>
       </c>
-      <c r="E87" s="2"/>
-      <c r="F87" s="3"/>
+      <c r="E87" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G87" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
@@ -3236,7 +3270,9 @@
       <c r="D91" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3258,7 +3294,9 @@
       <c r="D92" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E92" s="3"/>
+      <c r="E92" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>

</xml_diff>

<commit_message>
Added emissive Added subsurface Added near/far clip settings Added FOV settings Added directional light Added minimap Added LookAt Added terrain alignment with compute shader
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C748A0-1A15-4421-ACFD-A3EDB301CC10}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C233C3D-51F0-4D5F-9DE0-D46271858916}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="4788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="117">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -358,6 +358,27 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>Unity Quaternion Math: https://docs.unity3d.com/ScriptReference/Quaternion.html</t>
+  </si>
+  <si>
+    <t>Tutorial - Compute Shader Filters http://www.codinglabs.net/tutorial_compute_shaders_filters.aspx</t>
+  </si>
+  <si>
+    <t>Cascaded Shadow Maps https://docs.microsoft.com/en-us/windows/desktop/dxtecharts/cascaded-shadow-maps</t>
+  </si>
+  <si>
+    <t>OpenGL Physically Based Rendering : https://learnopengl.com/PBR/Theory</t>
+  </si>
+  <si>
+    <t>OpenGL Bloom :  https://learnopengl.com/Advanced-Lighting/Bloom</t>
+  </si>
+  <si>
+    <t>Sky HDRI Textures : https://hdrihaven.com/</t>
+  </si>
+  <si>
+    <t>Shadow Filtering : https://docs.cryengine.com/display/SDKDOC4/Shadows+in+CryENGINE</t>
   </si>
 </sst>
 </file>
@@ -948,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,11 +1108,11 @@
       </c>
       <c r="K4" s="16">
         <f>SUM(H6,I6,J6)</f>
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="L4" s="16">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1164,12 +1185,12 @@
       </c>
       <c r="J6" s="16">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="14">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1305,15 +1326,15 @@
       </c>
       <c r="H10" s="18">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="I10" s="18">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="J10" s="18">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1805,11 +1826,15 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
+      <c r="E29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G29" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1909,11 +1934,15 @@
       <c r="D33" s="5">
         <v>3</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G33" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2086,11 +2115,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G40" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2372,11 +2405,15 @@
       <c r="D52" s="5">
         <v>4</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="3"/>
+      <c r="E52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G52" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -2644,11 +2681,15 @@
       <c r="D64" s="5">
         <v>1</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="3"/>
+      <c r="E64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G64" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -2694,11 +2735,15 @@
       <c r="D66" s="5">
         <v>1</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="E66" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G66" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -2719,11 +2764,15 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="E67" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G67" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -3344,25 +3393,39 @@
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="11"/>
+      <c r="A97" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="11"/>
+      <c r="A98" s="11" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="11"/>
+      <c r="A99" s="11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="11"/>
+      <c r="A100" s="11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="11"/>
+      <c r="A101" s="11" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="11"/>
+      <c r="A102" s="11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="11"/>
+      <c r="A103" s="11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="11"/>
@@ -3431,7 +3494,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>